<commit_message>
MAIN: Work in progress.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szymo\Desktop\NPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F7D62-BD40-4406-8CBF-7352D0BE3940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BB6035-4C99-4967-BDD9-32F74172007E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>LP</t>
   </si>
@@ -51,12 +51,6 @@
     <t>MAUSER</t>
   </si>
   <si>
-    <t>TPS61088RHLR</t>
-  </si>
-  <si>
-    <t>https://www.mouser.pl/ProductDetail/Texas-Instruments/TPS61088RHLR?qs=MiqG6Kq1qKNjgpnslrNKug%3D%3D</t>
-  </si>
-  <si>
     <t>MCP73871-2CCI/ML</t>
   </si>
   <si>
@@ -69,12 +63,6 @@
     <t>https://www.mouser.pl/ProductDetail/Analog-Devices-Maxim-Integrated/MAX17048G+T10?qs=D7PJwyCwLAoGnnn8jEPRBQ%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.pl/ProductDetail/Murata-Electronics/NCU03XH103F6SRL?qs=%252BHhoWzUJg4LPq0SZgxAhJA%3D%3D</t>
-  </si>
-  <si>
-    <t>NCU03XH103F6SRL</t>
-  </si>
-  <si>
     <t>DOSTEPNE</t>
   </si>
   <si>
@@ -108,9 +96,6 @@
     <t>Termistor</t>
   </si>
   <si>
-    <t>Czujnik</t>
-  </si>
-  <si>
     <t>BMS</t>
   </si>
   <si>
@@ -127,6 +112,36 @@
   </si>
   <si>
     <t>87583-0010RHLF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.pl/ProductDetail/Amphenol-FCI/10118192-0001LF?qs=Ywefl8B65e5bHFoQtIudZg%3D%3D</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>Mirco USB B</t>
+  </si>
+  <si>
+    <t>USB A Female</t>
+  </si>
+  <si>
+    <t>https://www.mouser.pl/ProductDetail/Murata-Electronics/NCP18XH103E0SRB?qs=MIg4Wmhbclm5BvDMY8QW2Q%3D%3D</t>
+  </si>
+  <si>
+    <t>NCP18XH103E0SRB</t>
+  </si>
+  <si>
+    <t>Czujnik FG</t>
+  </si>
+  <si>
+    <t>Cewka</t>
+  </si>
+  <si>
+    <t>https://www.mouser.pl/ProductDetail/Wurth-Elektronik/744031010?qs=XJfXErqHgA7t3YCQkzSG5g%3D%3D</t>
+  </si>
+  <si>
+    <t>WE-TPC3816</t>
   </si>
 </sst>
 </file>
@@ -456,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L10"/>
+  <dimension ref="B2:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +487,7 @@
     <col min="8" max="8" width="43.109375" customWidth="1"/>
     <col min="9" max="9" width="9.88671875" customWidth="1"/>
     <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" customWidth="1"/>
     <col min="12" max="12" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -499,16 +514,16 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
@@ -516,64 +531,65 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>15.18</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="F3">
         <f>E3*D3</f>
-        <v>15.18</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4">
+        <f>B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>8.0399999999999991</v>
+        <v>9.85</v>
       </c>
       <c r="F4">
         <f>E4*D4</f>
-        <v>8.0399999999999991</v>
+        <v>9.85</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5">
-        <f>B4+1</f>
+        <f t="shared" ref="B5:B8" si="0">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" t="s">
@@ -583,11 +599,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>9.85</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="F5">
         <f>E5*D5</f>
-        <v>9.85</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -596,41 +612,34 @@
         <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6">
-        <f t="shared" ref="B6:B12" si="0">B5+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="F6">
-        <f>E6*D6</f>
-        <v>18.399999999999999</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" t="s">
-        <v>13</v>
+      <c r="H6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>1608</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
@@ -639,19 +648,25 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.96</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" t="s">
-        <v>14</v>
+      <c r="H7" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -660,80 +675,108 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <f>B6+1</f>
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8">
+      <c r="K11">
         <v>3216</v>
       </c>
-      <c r="L8">
+      <c r="L11">
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <f>B8+1</f>
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>B11+1</f>
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12">
         <v>3216</v>
       </c>
-      <c r="L9">
+      <c r="L12">
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3.96</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>744031010</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1" xr:uid="{68B7E947-357C-4566-9EA9-BF4D67B4055B}"/>
-    <hyperlink ref="H9" r:id="rId2" xr:uid="{B7E7471C-0D21-44DF-9C1B-81AD1F9AD4FF}"/>
+    <hyperlink ref="H11" r:id="rId1" xr:uid="{68B7E947-357C-4566-9EA9-BF4D67B4055B}"/>
+    <hyperlink ref="H12" r:id="rId2" xr:uid="{B7E7471C-0D21-44DF-9C1B-81AD1F9AD4FF}"/>
+    <hyperlink ref="H7" r:id="rId3" xr:uid="{F750C66B-1663-4FFF-85FD-DECBE4B2FCB7}"/>
+    <hyperlink ref="H8" r:id="rId4" xr:uid="{4E961C89-A0E6-4E3D-ABEC-5FB40750614F}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{14DDBE17-519B-4079-84CD-F58279D26EA9}"/>
+    <hyperlink ref="H15" r:id="rId6" xr:uid="{F962AE82-F9DA-4C68-BBEE-57FC37F55C32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAIN: PCB work in progress.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szymo\Desktop\NPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BB6035-4C99-4967-BDD9-32F74172007E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007F6EA9-6522-438B-A844-DE3229DC2E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>LP</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>WE-TPC3816</t>
+  </si>
+  <si>
+    <t>https://www.mouser.pl/ProductDetail/Keystone-Electronics/1042P?qs=g2rIOKKlpoboHyq0g1zn1A%3D%3D</t>
+  </si>
+  <si>
+    <t>1042P</t>
+  </si>
+  <si>
+    <t>Battery Holder</t>
   </si>
 </sst>
 </file>
@@ -474,7 +483,7 @@
   <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,7 +495,7 @@
     <col min="7" max="7" width="11.44140625" customWidth="1"/>
     <col min="8" max="8" width="43.109375" customWidth="1"/>
     <col min="9" max="9" width="9.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
     <col min="11" max="11" width="19.88671875" customWidth="1"/>
     <col min="12" max="12" width="18.5546875" customWidth="1"/>
   </cols>
@@ -691,6 +700,29 @@
       </c>
       <c r="J8" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>17.29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
MAIN: Wersja 2: poprawki sieci +5V_CHARGE.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szymo\Desktop\NPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007F6EA9-6522-438B-A844-DE3229DC2E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AE9A6F-C312-4982-BE6E-640B6E674AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,7 +715,7 @@
       <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="I9" t="s">
@@ -807,8 +807,9 @@
     <hyperlink ref="H8" r:id="rId4" xr:uid="{4E961C89-A0E6-4E3D-ABEC-5FB40750614F}"/>
     <hyperlink ref="H6" r:id="rId5" xr:uid="{14DDBE17-519B-4079-84CD-F58279D26EA9}"/>
     <hyperlink ref="H15" r:id="rId6" xr:uid="{F962AE82-F9DA-4C68-BBEE-57FC37F55C32}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{60D2B7B1-D3AA-4094-9175-7A74C253D395}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAIN: wersja 2, dodałem modele 3D.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szymo\Desktop\NPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AE9A6F-C312-4982-BE6E-640B6E674AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D10204-551F-4185-AA58-6D987ADB43CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1995" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>